<commit_message>
-Pushing the restructured architecture skeleton for selenium automation. -All libraries/dependencies are included in source path now. -Dependant resources are also added to the source.
</commit_message>
<xml_diff>
--- a/Resources/NavigationComponents.xlsx
+++ b/Resources/NavigationComponents.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t>ComponentName</t>
   </si>
@@ -28,6 +28,48 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>C- Click</t>
+  </si>
+  <si>
+    <t>D- Dropdown</t>
+  </si>
+  <si>
+    <t>Cclass</t>
+  </si>
+  <si>
+    <t>NA - Not Applicable</t>
+  </si>
+  <si>
+    <t>Cuvette</t>
+  </si>
+  <si>
+    <t>NanoVolume</t>
+  </si>
+  <si>
+    <t>StoreMethods</t>
+  </si>
+  <si>
+    <t>DataFiles</t>
+  </si>
+  <si>
+    <t>NucleicAcid</t>
+  </si>
+  <si>
+    <t>DyeLabeledNucleicAcid</t>
+  </si>
+  <si>
+    <t>ProteinUV</t>
+  </si>
+  <si>
+    <t>DyeLabeledProtein</t>
+  </si>
+  <si>
+    <t>GeneralMethods</t>
+  </si>
+  <si>
+    <t>NucleicAcid_SubTypes</t>
   </si>
 </sst>
 </file>
@@ -63,7 +105,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -366,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,21 +420,151 @@
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
clean up of driver Implementation
</commit_message>
<xml_diff>
--- a/Resources/NavigationComponents.xlsx
+++ b/Resources/NavigationComponents.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="17235" windowHeight="6210"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="12810" windowHeight="5760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -412,12 +413,12 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>